<commit_message>
Segunda edición de mi carpetita :'''v
</commit_message>
<xml_diff>
--- a/Tamaños de muestra.xlsx
+++ b/Tamaños de muestra.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JORGE\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>t</t>
   </si>
@@ -63,12 +58,24 @@
   </si>
   <si>
     <t>Costo</t>
+  </si>
+  <si>
+    <t>ADAD</t>
+  </si>
+  <si>
+    <t>Ojalá lo note</t>
+  </si>
+  <si>
+    <t>El gitHub</t>
+  </si>
+  <si>
+    <t>xdd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -412,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:J13"/>
+  <dimension ref="A2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D2" s="1">
         <v>0.98599999999999999</v>
       </c>
@@ -431,7 +438,7 @@
         <v>2.4576899999999999</v>
       </c>
     </row>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>1</v>
       </c>
@@ -439,12 +446,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>4</v>
       </c>
@@ -464,7 +471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E6" s="2">
         <v>0.05</v>
       </c>
@@ -487,7 +494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -507,7 +514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="2">
         <v>1.5</v>
       </c>
@@ -524,7 +531,10 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
@@ -541,7 +551,10 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
       <c r="E10" s="2">
         <v>2.5</v>
       </c>
@@ -558,7 +571,10 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
       <c r="E11" s="2">
         <v>3.5</v>
       </c>
@@ -575,7 +591,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
       <c r="E12" s="2">
         <v>4.2</v>
       </c>
@@ -592,7 +611,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" s="2">
         <v>5</v>
       </c>

</xml_diff>